<commit_message>
Test case 1 to Test case 9 all standAlone Scripts
</commit_message>
<xml_diff>
--- a/TestData/loginData.xlsx
+++ b/TestData/loginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\AdityaKunjir\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A949F0F-D9F2-4995-9E8B-4C9FFFFA65B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9562AAB-1F66-4088-9DA8-58F88A508FCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Failed! please enter strong password</t>
+  </si>
+  <si>
+    <t>aaa</t>
   </si>
 </sst>
 </file>
@@ -377,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -423,6 +426,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CAB5DFD0-A899-4EA1-B981-FCE5D87A916C}"/>

</xml_diff>